<commit_message>
updated to read files of the data automatically
</commit_message>
<xml_diff>
--- a/Dictionaries/20 July 2020_political dictionary.xlsx
+++ b/Dictionaries/20 July 2020_political dictionary.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\PycharmProjects\CapstoneProject\Dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\PycharmProjects\CapstoneProject\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBC9DED-F2FF-48E0-8307-D079EB6052D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FCCACC-D2FE-4F47-B8D1-DAFF4E79CEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -651,7 +662,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,8 +677,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,6 +704,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -699,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -708,6 +732,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -993,8 +1021,8 @@
   <dimension ref="A1:R73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,6 +1468,7 @@
       <c r="B31" s="2" t="s">
         <v>167</v>
       </c>
+      <c r="D31" s="4"/>
       <c r="N31" t="s">
         <v>1</v>
       </c>
@@ -1559,10 +1588,10 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="5" t="s">
         <v>176</v>
       </c>
       <c r="O41" t="s">

</xml_diff>